<commit_message>
Wstawione z LAB nr 1
</commit_message>
<xml_diff>
--- a/Small_Scripts/Ocenki/Wszystkie_Ocenki.xlsx
+++ b/Small_Scripts/Ocenki/Wszystkie_Ocenki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Python_Micro_Codes\Small_Scripts\Ocenki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54D3BF4-231C-4945-9133-52AFC4B03F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C1DF6B-93D0-4EB8-B63C-2351E8FE8ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53640" yWindow="2280" windowWidth="19440" windowHeight="15000" xr2:uid="{191E6661-648C-4C2D-8964-3C9A421F63BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{191E6661-648C-4C2D-8964-3C9A421F63BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="221">
   <si>
     <t>Lista ocen z zdalnego laboratorium CLF - Wydz. WIBHiŚ</t>
   </si>
@@ -1136,6 +1136,21 @@
   </si>
   <si>
     <t>Szarpak Anna</t>
+  </si>
+  <si>
+    <t>m,</t>
+  </si>
+  <si>
+    <t>1 - Wejściówka</t>
+  </si>
+  <si>
+    <t>1 - Sprawozdanie</t>
+  </si>
+  <si>
+    <t>- / 3 pkt</t>
+  </si>
+  <si>
+    <t>Ocena: 2 - 5</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1576,6 +1591,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -1891,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6F8E53-0F87-4890-8C97-73F30CDC1756}">
-  <dimension ref="A1:O120"/>
+  <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,15 +1923,27 @@
     <col min="7" max="7" width="10.7109375" style="27" customWidth="1"/>
     <col min="8" max="13" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q2" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="R2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1956,8 +1984,14 @@
       <c r="O3" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1982,8 +2016,10 @@
       <c r="O4" s="23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -2008,8 +2044,10 @@
       <c r="O5" s="24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -2031,8 +2069,10 @@
       <c r="K6" s="38"/>
       <c r="L6" s="38"/>
       <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -2052,8 +2092,10 @@
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
       <c r="M7" s="39"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -2075,8 +2117,10 @@
       <c r="K8" s="38"/>
       <c r="L8" s="38"/>
       <c r="M8" s="39"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -2098,8 +2142,10 @@
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
       <c r="M9" s="39"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -2121,8 +2167,10 @@
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
       <c r="M10" s="39"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -2144,8 +2192,10 @@
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="39"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -2167,8 +2217,10 @@
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="39"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -2190,8 +2242,10 @@
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="39"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -2213,8 +2267,10 @@
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="39"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -2236,8 +2292,10 @@
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
       <c r="M15" s="39"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -2259,8 +2317,10 @@
       <c r="K16" s="38"/>
       <c r="L16" s="38"/>
       <c r="M16" s="39"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -2282,8 +2342,10 @@
       <c r="K17" s="38"/>
       <c r="L17" s="38"/>
       <c r="M17" s="39"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -2305,8 +2367,10 @@
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="39"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -2328,8 +2392,10 @@
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="39"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -2351,8 +2417,10 @@
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="39"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -2374,8 +2442,10 @@
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="39"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -2397,8 +2467,10 @@
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="39"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -2420,8 +2492,10 @@
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="39"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -2443,8 +2517,10 @@
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="39"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -2466,8 +2542,10 @@
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
       <c r="M25" s="39"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -2489,8 +2567,10 @@
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
       <c r="M26" s="39"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>24</v>
       </c>
@@ -2512,8 +2592,10 @@
       <c r="K27" s="38"/>
       <c r="L27" s="38"/>
       <c r="M27" s="39"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -2533,8 +2615,10 @@
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
       <c r="M28" s="39"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -2558,8 +2642,10 @@
       <c r="K29" s="38"/>
       <c r="L29" s="38"/>
       <c r="M29" s="39"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -2583,8 +2669,10 @@
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="39"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>28</v>
       </c>
@@ -2606,8 +2694,10 @@
       <c r="K31" s="38"/>
       <c r="L31" s="38"/>
       <c r="M31" s="39"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>29</v>
       </c>
@@ -2631,8 +2721,10 @@
       <c r="K32" s="38"/>
       <c r="L32" s="38"/>
       <c r="M32" s="39"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>30</v>
       </c>
@@ -2654,8 +2746,10 @@
       <c r="K33" s="38"/>
       <c r="L33" s="38"/>
       <c r="M33" s="39"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -2677,8 +2771,14 @@
       <c r="K34" s="38"/>
       <c r="L34" s="38"/>
       <c r="M34" s="39"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q34" s="38">
+        <v>2.75</v>
+      </c>
+      <c r="R34" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>32</v>
       </c>
@@ -2702,8 +2802,10 @@
       <c r="K35" s="38"/>
       <c r="L35" s="38"/>
       <c r="M35" s="39"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>33</v>
       </c>
@@ -2727,8 +2829,10 @@
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
       <c r="M36" s="39"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>34</v>
       </c>
@@ -2752,8 +2856,10 @@
       <c r="K37" s="38"/>
       <c r="L37" s="38"/>
       <c r="M37" s="39"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -2777,8 +2883,10 @@
       <c r="K38" s="38"/>
       <c r="L38" s="38"/>
       <c r="M38" s="39"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q38" s="38"/>
+      <c r="R38" s="38"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>36</v>
       </c>
@@ -2802,8 +2910,10 @@
       <c r="K39" s="38"/>
       <c r="L39" s="38"/>
       <c r="M39" s="39"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -2827,8 +2937,10 @@
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
       <c r="M40" s="39"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>38</v>
       </c>
@@ -2850,8 +2962,10 @@
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
       <c r="M41" s="39"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39</v>
       </c>
@@ -2875,8 +2989,10 @@
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
       <c r="M42" s="39"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>40</v>
       </c>
@@ -2898,8 +3014,10 @@
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
       <c r="M43" s="39"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>41</v>
       </c>
@@ -2923,8 +3041,10 @@
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
       <c r="M44" s="39"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>42</v>
       </c>
@@ -2948,8 +3068,10 @@
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
       <c r="M45" s="39"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q45" s="38"/>
+      <c r="R45" s="38"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43</v>
       </c>
@@ -2971,8 +3093,10 @@
       <c r="K46" s="38"/>
       <c r="L46" s="38"/>
       <c r="M46" s="39"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q46" s="38"/>
+      <c r="R46" s="38"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44</v>
       </c>
@@ -2996,8 +3120,10 @@
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
       <c r="M47" s="39"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45</v>
       </c>
@@ -3019,8 +3145,10 @@
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
       <c r="M48" s="39"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>46</v>
       </c>
@@ -3044,8 +3172,10 @@
       <c r="K49" s="38"/>
       <c r="L49" s="38"/>
       <c r="M49" s="39"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -3069,8 +3199,10 @@
       <c r="K50" s="38"/>
       <c r="L50" s="38"/>
       <c r="M50" s="39"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q50" s="38"/>
+      <c r="R50" s="38"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>48</v>
       </c>
@@ -3094,8 +3226,10 @@
       <c r="K51" s="38"/>
       <c r="L51" s="38"/>
       <c r="M51" s="39"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q51" s="38"/>
+      <c r="R51" s="38"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>49</v>
       </c>
@@ -3119,8 +3253,10 @@
       <c r="K52" s="38"/>
       <c r="L52" s="38"/>
       <c r="M52" s="39"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>50</v>
       </c>
@@ -3144,8 +3280,10 @@
       <c r="K53" s="38"/>
       <c r="L53" s="38"/>
       <c r="M53" s="39"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q53" s="38"/>
+      <c r="R53" s="38"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>51</v>
       </c>
@@ -3167,8 +3305,10 @@
       <c r="K54" s="38"/>
       <c r="L54" s="38"/>
       <c r="M54" s="39"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q54" s="38"/>
+      <c r="R54" s="38"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>52</v>
       </c>
@@ -3190,8 +3330,10 @@
       <c r="K55" s="38"/>
       <c r="L55" s="38"/>
       <c r="M55" s="39"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>53</v>
       </c>
@@ -3213,8 +3355,10 @@
       <c r="K56" s="38"/>
       <c r="L56" s="38"/>
       <c r="M56" s="39"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q56" s="38"/>
+      <c r="R56" s="38"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>54</v>
       </c>
@@ -3234,8 +3378,10 @@
       <c r="K57" s="38"/>
       <c r="L57" s="38"/>
       <c r="M57" s="39"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>55</v>
       </c>
@@ -3255,8 +3401,10 @@
       <c r="K58" s="38"/>
       <c r="L58" s="38"/>
       <c r="M58" s="39"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q58" s="38"/>
+      <c r="R58" s="38"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>56</v>
       </c>
@@ -3278,8 +3426,10 @@
       <c r="K59" s="38"/>
       <c r="L59" s="38"/>
       <c r="M59" s="39"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q59" s="38"/>
+      <c r="R59" s="38"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>57</v>
       </c>
@@ -3301,8 +3451,10 @@
       <c r="K60" s="38"/>
       <c r="L60" s="38"/>
       <c r="M60" s="39"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q60" s="38"/>
+      <c r="R60" s="38"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>58</v>
       </c>
@@ -3326,8 +3478,10 @@
       <c r="K61" s="38"/>
       <c r="L61" s="38"/>
       <c r="M61" s="39"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q61" s="38"/>
+      <c r="R61" s="38"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>59</v>
       </c>
@@ -3351,8 +3505,10 @@
       <c r="K62" s="38"/>
       <c r="L62" s="38"/>
       <c r="M62" s="39"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q62" s="38"/>
+      <c r="R62" s="38"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>60</v>
       </c>
@@ -3374,8 +3530,14 @@
       <c r="K63" s="38"/>
       <c r="L63" s="38"/>
       <c r="M63" s="39"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q63" s="38">
+        <v>3</v>
+      </c>
+      <c r="R63" s="38">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>61</v>
       </c>
@@ -3397,8 +3559,10 @@
       <c r="K64" s="38"/>
       <c r="L64" s="38"/>
       <c r="M64" s="39"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q64" s="38"/>
+      <c r="R64" s="38"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>62</v>
       </c>
@@ -3420,8 +3584,10 @@
       <c r="K65" s="38"/>
       <c r="L65" s="38"/>
       <c r="M65" s="39"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q65" s="38"/>
+      <c r="R65" s="38"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>63</v>
       </c>
@@ -3443,8 +3609,14 @@
       <c r="K66" s="38"/>
       <c r="L66" s="38"/>
       <c r="M66" s="39"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q66" s="38">
+        <v>1.75</v>
+      </c>
+      <c r="R66" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>64</v>
       </c>
@@ -3466,8 +3638,10 @@
       <c r="K67" s="38"/>
       <c r="L67" s="38"/>
       <c r="M67" s="39"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q67" s="38"/>
+      <c r="R67" s="38"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>65</v>
       </c>
@@ -3489,8 +3663,14 @@
       <c r="K68" s="38"/>
       <c r="L68" s="38"/>
       <c r="M68" s="39"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q68" s="38">
+        <v>1</v>
+      </c>
+      <c r="R68" s="38">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>66</v>
       </c>
@@ -3512,8 +3692,10 @@
       <c r="K69" s="38"/>
       <c r="L69" s="38"/>
       <c r="M69" s="39"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q69" s="38"/>
+      <c r="R69" s="38"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>67</v>
       </c>
@@ -3533,8 +3715,10 @@
       <c r="K70" s="38"/>
       <c r="L70" s="38"/>
       <c r="M70" s="39"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q70" s="38"/>
+      <c r="R70" s="38"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>68</v>
       </c>
@@ -3556,8 +3740,10 @@
       <c r="K71" s="38"/>
       <c r="L71" s="38"/>
       <c r="M71" s="39"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q71" s="38"/>
+      <c r="R71" s="38"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>69</v>
       </c>
@@ -3579,8 +3765,14 @@
       <c r="K72" s="38"/>
       <c r="L72" s="38"/>
       <c r="M72" s="39"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q72" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="R72" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>70</v>
       </c>
@@ -3600,8 +3792,14 @@
       <c r="K73" s="38"/>
       <c r="L73" s="38"/>
       <c r="M73" s="39"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q73" s="38">
+        <v>3</v>
+      </c>
+      <c r="R73" s="38">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>71</v>
       </c>
@@ -3623,8 +3821,10 @@
       <c r="K74" s="38"/>
       <c r="L74" s="38"/>
       <c r="M74" s="39"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q74" s="38"/>
+      <c r="R74" s="38"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>72</v>
       </c>
@@ -3644,8 +3844,10 @@
       <c r="K75" s="38"/>
       <c r="L75" s="38"/>
       <c r="M75" s="39"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q75" s="38"/>
+      <c r="R75" s="38"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>73</v>
       </c>
@@ -3667,8 +3869,10 @@
       <c r="K76" s="38"/>
       <c r="L76" s="38"/>
       <c r="M76" s="39"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q76" s="38"/>
+      <c r="R76" s="38"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>74</v>
       </c>
@@ -3692,8 +3896,10 @@
       <c r="K77" s="38"/>
       <c r="L77" s="38"/>
       <c r="M77" s="39"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q77" s="38"/>
+      <c r="R77" s="38"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>75</v>
       </c>
@@ -3715,8 +3921,10 @@
       <c r="K78" s="38"/>
       <c r="L78" s="38"/>
       <c r="M78" s="39"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q78" s="38"/>
+      <c r="R78" s="38"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>76</v>
       </c>
@@ -3738,8 +3946,10 @@
       <c r="K79" s="38"/>
       <c r="L79" s="38"/>
       <c r="M79" s="39"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q79" s="38"/>
+      <c r="R79" s="38"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>77</v>
       </c>
@@ -3761,8 +3971,10 @@
       <c r="K80" s="38"/>
       <c r="L80" s="38"/>
       <c r="M80" s="39"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q80" s="38"/>
+      <c r="R80" s="38"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>78</v>
       </c>
@@ -3784,8 +3996,10 @@
       <c r="K81" s="38"/>
       <c r="L81" s="38"/>
       <c r="M81" s="39"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q81" s="38"/>
+      <c r="R81" s="38"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>79</v>
       </c>
@@ -3807,8 +4021,10 @@
       <c r="K82" s="38"/>
       <c r="L82" s="38"/>
       <c r="M82" s="39"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q82" s="38"/>
+      <c r="R82" s="38"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>80</v>
       </c>
@@ -3830,8 +4046,10 @@
       <c r="K83" s="38"/>
       <c r="L83" s="38"/>
       <c r="M83" s="39"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q83" s="38"/>
+      <c r="R83" s="38"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>81</v>
       </c>
@@ -3853,8 +4071,10 @@
       <c r="K84" s="38"/>
       <c r="L84" s="38"/>
       <c r="M84" s="39"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q84" s="38"/>
+      <c r="R84" s="38"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>82</v>
       </c>
@@ -3876,8 +4096,10 @@
       <c r="K85" s="38"/>
       <c r="L85" s="38"/>
       <c r="M85" s="39"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q85" s="38"/>
+      <c r="R85" s="38"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>83</v>
       </c>
@@ -3899,8 +4121,10 @@
       <c r="K86" s="38"/>
       <c r="L86" s="38"/>
       <c r="M86" s="39"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q86" s="38"/>
+      <c r="R86" s="38"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>84</v>
       </c>
@@ -3922,8 +4146,10 @@
       <c r="K87" s="38"/>
       <c r="L87" s="38"/>
       <c r="M87" s="39"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q87" s="38"/>
+      <c r="R87" s="38"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>85</v>
       </c>
@@ -3945,8 +4171,10 @@
       <c r="K88" s="38"/>
       <c r="L88" s="38"/>
       <c r="M88" s="39"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q88" s="38"/>
+      <c r="R88" s="38"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>86</v>
       </c>
@@ -3968,8 +4196,10 @@
       <c r="K89" s="38"/>
       <c r="L89" s="38"/>
       <c r="M89" s="39"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q89" s="38"/>
+      <c r="R89" s="38"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>87</v>
       </c>
@@ -3991,8 +4221,14 @@
       <c r="K90" s="38"/>
       <c r="L90" s="38"/>
       <c r="M90" s="39"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q90" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="R90" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>88</v>
       </c>
@@ -4014,8 +4250,10 @@
       <c r="K91" s="38"/>
       <c r="L91" s="38"/>
       <c r="M91" s="39"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q91" s="38"/>
+      <c r="R91" s="38"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>89</v>
       </c>
@@ -4037,8 +4275,14 @@
       <c r="K92" s="38"/>
       <c r="L92" s="38"/>
       <c r="M92" s="39"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q92" s="38">
+        <v>3</v>
+      </c>
+      <c r="R92" s="38">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>90</v>
       </c>
@@ -4060,8 +4304,14 @@
       <c r="K93" s="38"/>
       <c r="L93" s="38"/>
       <c r="M93" s="39"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q93" s="38">
+        <v>1.75</v>
+      </c>
+      <c r="R93" s="38">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>91</v>
       </c>
@@ -4083,8 +4333,10 @@
       <c r="K94" s="38"/>
       <c r="L94" s="38"/>
       <c r="M94" s="39"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q94" s="38"/>
+      <c r="R94" s="38"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>92</v>
       </c>
@@ -4104,8 +4356,10 @@
       <c r="K95" s="38"/>
       <c r="L95" s="38"/>
       <c r="M95" s="39"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q95" s="38"/>
+      <c r="R95" s="38"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>93</v>
       </c>
@@ -4127,8 +4381,10 @@
       <c r="K96" s="38"/>
       <c r="L96" s="38"/>
       <c r="M96" s="39"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q96" s="38"/>
+      <c r="R96" s="38"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>94</v>
       </c>
@@ -4150,8 +4406,10 @@
       <c r="K97" s="38"/>
       <c r="L97" s="38"/>
       <c r="M97" s="39"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q97" s="38"/>
+      <c r="R97" s="38"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>95</v>
       </c>
@@ -4173,8 +4431,10 @@
       <c r="K98" s="38"/>
       <c r="L98" s="38"/>
       <c r="M98" s="39"/>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q98" s="38"/>
+      <c r="R98" s="38"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>96</v>
       </c>
@@ -4196,8 +4456,10 @@
       <c r="K99" s="38"/>
       <c r="L99" s="38"/>
       <c r="M99" s="39"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q99" s="38"/>
+      <c r="R99" s="38"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>97</v>
       </c>
@@ -4219,8 +4481,10 @@
       <c r="K100" s="38"/>
       <c r="L100" s="38"/>
       <c r="M100" s="39"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q100" s="38"/>
+      <c r="R100" s="38"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>98</v>
       </c>
@@ -4244,8 +4508,10 @@
       <c r="K101" s="38"/>
       <c r="L101" s="38"/>
       <c r="M101" s="39"/>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q101" s="38"/>
+      <c r="R101" s="38"/>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>99</v>
       </c>
@@ -4267,8 +4533,10 @@
       <c r="K102" s="38"/>
       <c r="L102" s="38"/>
       <c r="M102" s="39"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q102" s="38"/>
+      <c r="R102" s="38"/>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>100</v>
       </c>
@@ -4292,8 +4560,10 @@
       <c r="K103" s="38"/>
       <c r="L103" s="38"/>
       <c r="M103" s="39"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q103" s="38"/>
+      <c r="R103" s="38"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>101</v>
       </c>
@@ -4315,8 +4585,10 @@
       <c r="K104" s="38"/>
       <c r="L104" s="38"/>
       <c r="M104" s="39"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q104" s="38"/>
+      <c r="R104" s="38"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>102</v>
       </c>
@@ -4336,8 +4608,10 @@
       <c r="K105" s="38"/>
       <c r="L105" s="38"/>
       <c r="M105" s="39"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q105" s="38"/>
+      <c r="R105" s="38"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>103</v>
       </c>
@@ -4361,8 +4635,10 @@
       <c r="K106" s="38"/>
       <c r="L106" s="38"/>
       <c r="M106" s="39"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q106" s="38"/>
+      <c r="R106" s="38"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>104</v>
       </c>
@@ -4384,8 +4660,10 @@
       <c r="K107" s="38"/>
       <c r="L107" s="38"/>
       <c r="M107" s="39"/>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q107" s="38"/>
+      <c r="R107" s="38"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>105</v>
       </c>
@@ -4407,8 +4685,10 @@
       <c r="K108" s="38"/>
       <c r="L108" s="38"/>
       <c r="M108" s="39"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q108" s="38"/>
+      <c r="R108" s="38"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>106</v>
       </c>
@@ -4432,8 +4712,10 @@
       <c r="K109" s="38"/>
       <c r="L109" s="38"/>
       <c r="M109" s="39"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q109" s="38"/>
+      <c r="R109" s="38"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>107</v>
       </c>
@@ -4455,8 +4737,10 @@
       <c r="K110" s="38"/>
       <c r="L110" s="38"/>
       <c r="M110" s="39"/>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q110" s="38"/>
+      <c r="R110" s="38"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>108</v>
       </c>
@@ -4480,8 +4764,10 @@
       <c r="K111" s="38"/>
       <c r="L111" s="38"/>
       <c r="M111" s="39"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q111" s="38"/>
+      <c r="R111" s="38"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>109</v>
       </c>
@@ -4505,8 +4791,10 @@
       <c r="K112" s="38"/>
       <c r="L112" s="38"/>
       <c r="M112" s="39"/>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q112" s="38"/>
+      <c r="R112" s="38"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>110</v>
       </c>
@@ -4530,8 +4818,10 @@
       <c r="K113" s="38"/>
       <c r="L113" s="38"/>
       <c r="M113" s="39"/>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q113" s="38"/>
+      <c r="R113" s="38"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>111</v>
       </c>
@@ -4555,8 +4845,10 @@
       <c r="K114" s="38"/>
       <c r="L114" s="38"/>
       <c r="M114" s="39"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q114" s="38"/>
+      <c r="R114" s="38"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>112</v>
       </c>
@@ -4580,8 +4872,10 @@
       <c r="K115" s="38"/>
       <c r="L115" s="38"/>
       <c r="M115" s="39"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q115" s="38"/>
+      <c r="R115" s="38"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>113</v>
       </c>
@@ -4605,8 +4899,10 @@
       <c r="K116" s="38"/>
       <c r="L116" s="38"/>
       <c r="M116" s="39"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q116" s="38"/>
+      <c r="R116" s="38"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E117" s="41"/>
       <c r="F117" s="42"/>
       <c r="G117" s="37"/>
@@ -4616,8 +4912,10 @@
       <c r="K117" s="38"/>
       <c r="L117" s="38"/>
       <c r="M117" s="39"/>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q117" s="38"/>
+      <c r="R117" s="38"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B118" s="13" t="s">
         <v>183</v>
       </c>
@@ -4636,8 +4934,10 @@
       <c r="K118" s="38"/>
       <c r="L118" s="38"/>
       <c r="M118" s="39"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q118" s="38"/>
+      <c r="R118" s="38"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B119" s="13" t="s">
         <v>184</v>
       </c>
@@ -4656,8 +4956,10 @@
       <c r="K119" s="38"/>
       <c r="L119" s="38"/>
       <c r="M119" s="39"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q119" s="38"/>
+      <c r="R119" s="38"/>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
         <v>185</v>
       </c>
@@ -4676,6 +4978,8 @@
       <c r="K120" s="46"/>
       <c r="L120" s="46"/>
       <c r="M120" s="47"/>
+      <c r="Q120" s="38"/>
+      <c r="R120" s="38"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F116">
@@ -4896,6 +5200,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101002AA3312276810947AF3FA964E66FF2FE" ma:contentTypeVersion="2" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="04d955c0d9ad59419875f3f17abd1d51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02c6c4a4-04be-4aab-8ad6-059ab683dcdc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd66fb7ecdca5f068b578c4de9bc4241" ns2:_="">
     <xsd:import namespace="02c6c4a4-04be-4aab-8ad6-059ab683dcdc"/>
@@ -5027,12 +5337,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7AA4A0B-56E6-4C5A-871F-EB085BAC05C4}">
   <ds:schemaRefs>
@@ -5042,6 +5346,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4C885C8-7E0F-464C-B85F-262DC4145968}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82030813-5E6E-42B9-A784-90825896D5DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5057,13 +5370,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4C885C8-7E0F-464C-B85F-262DC4145968}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>